<commit_message>
Data Analysis result commit 1
- Analysis results about sampling compoisitions
- Definitions & Approaches charts
- First analisys about trade-offs
</commit_message>
<xml_diff>
--- a/Analisi dei dati/Ferrara/Datasets/Post Processing/RQ1.xlsx
+++ b/Analisi dei dati/Ferrara/Datasets/Post Processing/RQ1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carmi\Desktop\Tesi Magistrale\TesiFairness\Analisi dei dati\Ferrara\Datasets\Post Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865A82EE-47EF-4575-A31F-D7DE4460482C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E572698-C27D-4DDA-BA4C-5FD983810276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4041,7 +4041,7 @@
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F1" activeCellId="1" sqref="E1:E1048576 F1:F1048576"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4179,7 +4179,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -5413,7 +5413,7 @@
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>